<commit_message>
Random number of neurons and learning rate, add surrogate and confusion matrix
</commit_message>
<xml_diff>
--- a/Classification_model/classification_nets_empty.xlsx
+++ b/Classification_model/classification_nets_empty.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,77 +452,97 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>layer_init_size</t>
+          <t>layers_size</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>layers_size</t>
+          <t>net_param</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>net_param</t>
+          <t>criterion</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>criterion</t>
+          <t>learning_rate</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>learning_rate</t>
+          <t>optimizer</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>optimizer</t>
+          <t>epochs</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>epochs</t>
+          <t>vali_best_epoch</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>vali_best_epoch</t>
+          <t>vali_best_acc</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>vali_best_acc</t>
+          <t>vali_best_loss</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>vali_best_loss</t>
+          <t>vali_best_R</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>vali_best_R</t>
+          <t>vali_sur_acc</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
+          <t>vali_sur_loss</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>vali_sur_R</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
           <t>test_acc</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>test_loss</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>test_R</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>predicted</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>c_matrix</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>c_matrix_perc</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Net analysis, Load selected nets, Loop vali_confusion_matrix
</commit_message>
<xml_diff>
--- a/Classification_model/classification_nets_empty.xlsx
+++ b/Classification_model/classification_nets_empty.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,32 +517,42 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
+          <t>vali_c_matrix</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>vali_c_matrix_perc</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
           <t>test_acc</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>test_loss</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>test_R</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>predicted</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>c_matrix</t>
-        </is>
-      </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>c_matrix_perc</t>
+          <t>test_predicted</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>test_c_matrix</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>test_c_matrix_perc</t>
         </is>
       </c>
     </row>

</xml_diff>